<commit_message>
Update Voter Access-Comp Rankings.xlsx
</commit_message>
<xml_diff>
--- a/Voter Access-Comp Rankings.xlsx
+++ b/Voter Access-Comp Rankings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mendelzecher/Documents/GitHub/mz2733/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FDDB2D7-73E8-EC40-AF28-E3F2EF46E540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{354AA87F-E1E4-5343-BEF2-1EC8DE1A7B1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5700" yWindow="460" windowWidth="22720" windowHeight="16520" xr2:uid="{1EA0DDB8-C307-DC47-A298-7BB04BBB4F7C}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="54">
   <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>AL</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>IO</t>
   </si>
   <si>
-    <t>STATE #</t>
-  </si>
-  <si>
     <t>YEAR</t>
   </si>
   <si>
@@ -198,6 +192,12 @@
   </si>
   <si>
     <t>Percent Diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State </t>
+  </si>
+  <si>
+    <t>State ABB</t>
   </si>
 </sst>
 </file>
@@ -578,31 +578,31 @@
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>38</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <v>41</v>
@@ -674,7 +674,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6">
         <v>56</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>55</v>
@@ -710,7 +710,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <v>19</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>27</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>33</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>50</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <v>37</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>9</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>53</v>
@@ -890,7 +890,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>31</v>
@@ -908,7 +908,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>24</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20">
         <v>49</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>17</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22">
         <v>15</v>
@@ -980,7 +980,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23">
         <v>54</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>34</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25">
         <v>25</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -1052,7 +1052,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27">
         <v>46</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28">
         <v>12</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29">
         <v>20</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30">
         <v>32</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32">
         <v>13</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>40</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34">
         <v>10</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35">
         <v>22</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36">
         <v>36</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>44</v>
@@ -1268,7 +1268,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B39">
         <v>35</v>
@@ -1286,7 +1286,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40">
         <v>42</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B41">
         <v>5</v>
@@ -1322,7 +1322,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B42">
         <v>26</v>
@@ -1340,7 +1340,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43">
         <v>29</v>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44">
         <v>16</v>
@@ -1376,7 +1376,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45">
         <v>48</v>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B46">
         <v>21</v>
@@ -1412,7 +1412,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B47">
         <v>39</v>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B48">
         <v>47</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B49">
         <v>45</v>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50">
         <v>51</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B51">
         <v>28</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B52">
         <v>38</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B53">
         <v>23</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54">
         <v>16</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B55">
         <v>41</v>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B56">
         <v>56</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B57">
         <v>55</v>
@@ -1610,7 +1610,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B58">
         <v>19</v>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B59">
         <v>27</v>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B60">
         <v>33</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -1682,7 +1682,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B62">
         <v>6</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B63">
         <v>50</v>
@@ -1718,7 +1718,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B64">
         <v>30</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B65">
         <v>37</v>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B66">
         <v>9</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B67">
         <v>53</v>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B68">
         <v>31</v>
@@ -1808,7 +1808,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B69">
         <v>24</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B70">
         <v>49</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B71">
         <v>17</v>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B72">
         <v>15</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B73">
         <v>54</v>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B74">
         <v>34</v>
@@ -1916,7 +1916,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B75">
         <v>25</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B77">
         <v>46</v>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B78">
         <v>12</v>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B79">
         <v>20</v>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B80">
         <v>32</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B81">
         <v>4</v>
@@ -2042,7 +2042,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B82">
         <v>13</v>
@@ -2060,7 +2060,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B83">
         <v>40</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B84">
         <v>10</v>
@@ -2096,7 +2096,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B85">
         <v>22</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B86">
         <v>36</v>
@@ -2132,7 +2132,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B88">
         <v>44</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B89">
         <v>35</v>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B90">
         <v>42</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B91">
         <v>5</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B92">
         <v>26</v>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B93">
         <v>29</v>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B94">
         <v>16</v>
@@ -2276,7 +2276,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B95">
         <v>48</v>
@@ -2294,7 +2294,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B96">
         <v>21</v>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B97">
         <v>39</v>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B98">
         <v>47</v>
@@ -2348,7 +2348,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B99">
         <v>45</v>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B100">
         <v>51</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B101">
         <v>28</v>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B102">
         <v>38</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B103">
         <v>23</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B104">
         <v>16</v>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B105">
         <v>41</v>
@@ -2474,7 +2474,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B106">
         <v>56</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B107">
         <v>55</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B108">
         <v>19</v>
@@ -2528,7 +2528,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B109">
         <v>27</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B110">
         <v>33</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B111">
         <v>8</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B112">
         <v>6</v>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B113">
         <v>50</v>
@@ -2618,7 +2618,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B114">
         <v>30</v>
@@ -2636,7 +2636,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B115">
         <v>37</v>
@@ -2654,7 +2654,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B116">
         <v>9</v>
@@ -2672,7 +2672,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B117">
         <v>53</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B118">
         <v>31</v>
@@ -2708,7 +2708,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B119">
         <v>24</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B120">
         <v>49</v>
@@ -2744,7 +2744,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B121">
         <v>17</v>
@@ -2762,7 +2762,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B122">
         <v>15</v>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B123">
         <v>54</v>
@@ -2798,7 +2798,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B124">
         <v>34</v>
@@ -2816,7 +2816,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B125">
         <v>25</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B126">
         <v>2</v>
@@ -2852,7 +2852,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B127">
         <v>46</v>
@@ -2870,7 +2870,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B128">
         <v>12</v>
@@ -2888,7 +2888,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B129">
         <v>20</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B130">
         <v>32</v>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B131">
         <v>4</v>
@@ -2942,7 +2942,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B132">
         <v>13</v>
@@ -2960,7 +2960,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B133">
         <v>40</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B134">
         <v>10</v>
@@ -2996,7 +2996,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B135">
         <v>22</v>
@@ -3014,7 +3014,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B136">
         <v>36</v>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -3050,7 +3050,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B138">
         <v>44</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B139">
         <v>35</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B140">
         <v>42</v>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B141">
         <v>5</v>
@@ -3122,7 +3122,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B142">
         <v>26</v>
@@ -3140,7 +3140,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B143">
         <v>29</v>
@@ -3158,7 +3158,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B144">
         <v>16</v>
@@ -3176,7 +3176,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B145">
         <v>48</v>
@@ -3194,7 +3194,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B146">
         <v>21</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B147">
         <v>39</v>
@@ -3230,7 +3230,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B148">
         <v>47</v>
@@ -3248,7 +3248,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B149">
         <v>45</v>
@@ -3266,7 +3266,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B150">
         <v>51</v>
@@ -3284,7 +3284,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B151">
         <v>28</v>
@@ -3302,7 +3302,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B152">
         <v>38</v>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B153">
         <v>23</v>
@@ -3338,7 +3338,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B154">
         <v>16</v>
@@ -3356,7 +3356,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B155">
         <v>41</v>
@@ -3374,7 +3374,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B156">
         <v>56</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B157">
         <v>55</v>
@@ -3410,7 +3410,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B158">
         <v>19</v>
@@ -3428,7 +3428,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B159">
         <v>27</v>
@@ -3446,7 +3446,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B160">
         <v>33</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B161">
         <v>8</v>
@@ -3482,7 +3482,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B162">
         <v>6</v>
@@ -3500,7 +3500,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B163">
         <v>50</v>
@@ -3518,7 +3518,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B164">
         <v>30</v>
@@ -3536,7 +3536,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B165">
         <v>37</v>
@@ -3554,7 +3554,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B166">
         <v>9</v>
@@ -3572,7 +3572,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B167">
         <v>53</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B168">
         <v>31</v>
@@ -3608,7 +3608,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B169">
         <v>24</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B170">
         <v>49</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B171">
         <v>17</v>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B172">
         <v>15</v>
@@ -3680,7 +3680,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B173">
         <v>54</v>
@@ -3698,7 +3698,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B174">
         <v>34</v>
@@ -3716,7 +3716,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B175">
         <v>25</v>
@@ -3734,7 +3734,7 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B176">
         <v>2</v>
@@ -3752,7 +3752,7 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B177">
         <v>46</v>
@@ -3770,7 +3770,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B178">
         <v>12</v>
@@ -3788,7 +3788,7 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B179">
         <v>20</v>
@@ -3806,7 +3806,7 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B180">
         <v>32</v>
@@ -3824,7 +3824,7 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B181">
         <v>4</v>
@@ -3842,7 +3842,7 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B182">
         <v>13</v>
@@ -3860,7 +3860,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B183">
         <v>40</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B184">
         <v>10</v>
@@ -3896,7 +3896,7 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B185">
         <v>22</v>
@@ -3914,7 +3914,7 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B186">
         <v>36</v>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B187">
         <v>1</v>
@@ -3950,7 +3950,7 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B188">
         <v>44</v>
@@ -3968,7 +3968,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B189">
         <v>35</v>
@@ -3986,7 +3986,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B190">
         <v>42</v>
@@ -4004,7 +4004,7 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B191">
         <v>5</v>
@@ -4022,7 +4022,7 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B192">
         <v>26</v>
@@ -4040,7 +4040,7 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B193">
         <v>29</v>
@@ -4058,7 +4058,7 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B194">
         <v>16</v>
@@ -4076,7 +4076,7 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B195">
         <v>48</v>
@@ -4094,7 +4094,7 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B196">
         <v>21</v>
@@ -4112,7 +4112,7 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B197">
         <v>39</v>
@@ -4130,7 +4130,7 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B198">
         <v>47</v>
@@ -4148,7 +4148,7 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B199">
         <v>45</v>
@@ -4166,7 +4166,7 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B200">
         <v>51</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B201">
         <v>28</v>

</xml_diff>